<commit_message>
mouse hover and frame testcases
</commit_message>
<xml_diff>
--- a/RunManager.xlsx
+++ b/RunManager.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="31">
   <si>
     <t>S.No</t>
   </si>
@@ -80,6 +80,30 @@
   </si>
   <si>
     <t>features/UnitTestCases.feature:27</t>
+  </si>
+  <si>
+    <t>Web Table Handling_Get coursename based on price</t>
+  </si>
+  <si>
+    <t>features/UnitTestCases.feature:31</t>
+  </si>
+  <si>
+    <t>Fixed Web Table Handling_Validate total price</t>
+  </si>
+  <si>
+    <t>features/UnitTestCases.feature:35</t>
+  </si>
+  <si>
+    <t>Mouse Hover validation</t>
+  </si>
+  <si>
+    <t>features/UnitTestCases.feature:39</t>
+  </si>
+  <si>
+    <t>Frame Validation</t>
+  </si>
+  <si>
+    <t>features/UnitTestCases.feature:43</t>
   </si>
   <si>
     <t>Yes</t>
@@ -475,16 +499,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F8"/>
+  <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView workbookViewId="0" zoomScale="100" zoomScaleNormal="100">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="0.35" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="8.7265625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="39.453125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="55.36328125" style="1" customWidth="1"/>
     <col min="3" max="3" width="36.90625" style="1" customWidth="1"/>
     <col min="4" max="4" width="10.26953125" style="1" customWidth="1"/>
     <col min="5" max="5" width="15.54296875" style="1" customWidth="1"/>
@@ -630,10 +654,78 @@
       <c r="C8" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="D8" s="3" t="s">
+      <c r="D8" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" ht="14.5" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>8</v>
+      </c>
+      <c r="B9" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="E8" s="1" t="s">
+      <c r="C9" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" ht="14.5" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <v>9</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" ht="14.5" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
+        <v>10</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" ht="14.5" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
+        <v>11</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="E12" s="1" t="s">
         <v>9</v>
       </c>
     </row>

</xml_diff>